<commit_message>
added more tasks to list
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vertex42.com\Documents\VERTEX42\TEMPLATES\TEMPLATE - Lists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanes\Documents\Projects\Lightning Trigger\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2689F4C4-A791-40F2-8397-517E32D93113}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25680" windowHeight="11685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5568" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTaskList" sheetId="7" r:id="rId1"/>
@@ -22,17 +23,23 @@
     <definedName name="vertex42_id" hidden="1">"project-task-list-template.xlsx"</definedName>
     <definedName name="vertex42_title" hidden="1">"Task List Template"</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>PRIORITY</t>
   </si>
@@ -82,15 +89,6 @@
     <t>% COMPLETE</t>
   </si>
   <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Task 2</t>
-  </si>
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
     <t>DONE</t>
   </si>
   <si>
@@ -101,9 +99,6 @@
   </si>
   <si>
     <t>HIGH</t>
-  </si>
-  <si>
-    <t>MEDIUM</t>
   </si>
   <si>
     <t>LOW</t>
@@ -145,9 +140,6 @@
   </si>
   <si>
     <t>END</t>
-  </si>
-  <si>
-    <t>PROJECT TASK LIST</t>
   </si>
   <si>
     <t>Learn More</t>
@@ -196,14 +188,35 @@
   <si>
     <t>The Done column is updated automatically. When you enter 100% in the % Complete column, the checkmark should appear in the Done column. You can use the drop-down in the Done column if you prefer.</t>
   </si>
+  <si>
+    <t>LIGHTNING TRIGGER</t>
+  </si>
+  <si>
+    <t>HARDWARE</t>
+  </si>
+  <si>
+    <t>SOFTWARE</t>
+  </si>
+  <si>
+    <t>Draw Schematic</t>
+  </si>
+  <si>
+    <t>Layout PCB</t>
+  </si>
+  <si>
+    <t>Assemble PCB</t>
+  </si>
+  <si>
+    <t>Port software off Arduino (To Atmel Studio)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -410,7 +423,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -530,7 +543,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -560,7 +573,7 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -575,7 +588,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -753,7 +766,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1055,7 +1068,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="ToDoList" pivot="0" count="9">
+    <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="36"/>
       <tableStyleElement type="headerRow" dxfId="35"/>
       <tableStyleElement type="totalRow" dxfId="34"/>
@@ -1134,22 +1147,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table137" displayName="Table137" ref="A5:K31" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A5:K31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table137" displayName="Table137" ref="A5:K31" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A5:K31" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="TASK" dataDxfId="10"/>
-    <tableColumn id="8" name="OWNER" dataDxfId="9"/>
-    <tableColumn id="7" name="PRIORITY" dataDxfId="8"/>
-    <tableColumn id="4" name="START" dataDxfId="7"/>
-    <tableColumn id="5" name="END" dataDxfId="6"/>
-    <tableColumn id="2" name="% COMPLETE" dataDxfId="5" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="DONE" dataDxfId="4" dataCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TASK" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="OWNER" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="PRIORITY" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="START" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="END" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="% COMPLETE" dataDxfId="5" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DONE" dataDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>IF(F6&gt;=1,1,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="BUDGET" dataDxfId="3" dataCellStyle="Percent"/>
-    <tableColumn id="11" name="EST._x000a_HOURS" dataDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="12" name="ACTUAL_x000a_HOURS" dataDxfId="1" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="NOTES" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="BUDGET" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="EST._x000a_HOURS" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ACTUAL_x000a_HOURS" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="NOTES" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="ToDoList" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -1417,32 +1430,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.25" customWidth="1"/>
+    <col min="1" max="1" width="22.19921875" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
-    <col min="3" max="3" width="10.125" customWidth="1"/>
-    <col min="4" max="4" width="11.125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="11.125" customWidth="1"/>
-    <col min="6" max="6" width="14.625" customWidth="1"/>
-    <col min="7" max="7" width="6.25" customWidth="1"/>
-    <col min="8" max="10" width="10.25" customWidth="1"/>
-    <col min="11" max="11" width="20.125" customWidth="1"/>
+    <col min="3" max="3" width="10.09765625" customWidth="1"/>
+    <col min="4" max="4" width="11.09765625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="11.09765625" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" customWidth="1"/>
+    <col min="7" max="7" width="6.19921875" customWidth="1"/>
+    <col min="8" max="10" width="10.19921875" customWidth="1"/>
+    <col min="11" max="11" width="20.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1455,33 +1468,33 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H2" s="20" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M2" s="23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="54" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" s="55">
         <v>42736</v>
       </c>
       <c r="G3" s="54" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H3" s="56">
         <f>SUM(Table137[BUDGET])</f>
-        <v>1650</v>
+        <v>0</v>
       </c>
       <c r="I3" s="57">
         <f>SUM(Table137[EST.
@@ -1497,47 +1510,47 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M4" s="23"/>
     </row>
-    <row r="5" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>25</v>
-      </c>
       <c r="C5" s="37" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F5" s="36" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H5" s="44" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I5" s="36" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K5" s="13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="53" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B6" s="45"/>
       <c r="C6" s="46"/>
@@ -1553,92 +1566,72 @@
       <c r="J6" s="52"/>
       <c r="K6" s="46"/>
     </row>
-    <row r="7" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="17">
-        <v>42737</v>
-      </c>
-      <c r="E7" s="25">
-        <v>42738</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="28">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
       <c r="G7" s="30">
         <v>0</v>
       </c>
-      <c r="H7" s="41">
-        <v>1000</v>
-      </c>
+      <c r="H7" s="41"/>
       <c r="I7" s="39"/>
       <c r="J7" s="39"/>
       <c r="K7" s="12"/>
     </row>
-    <row r="8" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="17">
-        <v>42737</v>
-      </c>
-      <c r="E8" s="25">
-        <f ca="1">TODAY()</f>
-        <v>42761</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="28">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="G8" s="30">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H8" s="41">
-        <v>400</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H8" s="41"/>
       <c r="I8" s="39"/>
       <c r="J8" s="39"/>
       <c r="K8" s="12"/>
     </row>
-    <row r="9" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="17">
-        <v>42737</v>
-      </c>
-      <c r="E9" s="25">
-        <f ca="1">TODAY()+2</f>
-        <v>42763</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="25"/>
       <c r="F9" s="28">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G9" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H9" s="41">
-        <v>250</v>
-      </c>
+      <c r="H9" s="41"/>
       <c r="I9" s="39"/>
       <c r="J9" s="39"/>
       <c r="K9" s="12"/>
     </row>
-    <row r="10" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="12"/>
@@ -1654,9 +1647,9 @@
       <c r="J10" s="39"/>
       <c r="K10" s="12"/>
     </row>
-    <row r="11" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B11" s="45"/>
       <c r="C11" s="46"/>
@@ -1672,7 +1665,7 @@
       <c r="J11" s="52"/>
       <c r="K11" s="46"/>
     </row>
-    <row r="12" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
       <c r="C12" s="12"/>
@@ -1688,7 +1681,7 @@
       <c r="J12" s="39"/>
       <c r="K12" s="12"/>
     </row>
-    <row r="13" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="12"/>
@@ -1704,7 +1697,7 @@
       <c r="J13" s="39"/>
       <c r="K13" s="12"/>
     </row>
-    <row r="14" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
@@ -1720,13 +1713,19 @@
       <c r="J14" s="39"/>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
+    <row r="15" spans="1:13" s="15" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
+      <c r="C15" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="D15" s="18"/>
       <c r="E15" s="26"/>
-      <c r="F15" s="28"/>
+      <c r="F15" s="28">
+        <v>0</v>
+      </c>
       <c r="G15" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1736,9 +1735,9 @@
       <c r="J15" s="39"/>
       <c r="K15" s="12"/>
     </row>
-    <row r="16" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="53" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B16" s="45"/>
       <c r="C16" s="46"/>
@@ -1754,7 +1753,7 @@
       <c r="J16" s="52"/>
       <c r="K16" s="46"/>
     </row>
-    <row r="17" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
       <c r="C17" s="12"/>
@@ -1770,7 +1769,7 @@
       <c r="J17" s="39"/>
       <c r="K17" s="12"/>
     </row>
-    <row r="18" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="12"/>
@@ -1786,7 +1785,7 @@
       <c r="J18" s="40"/>
       <c r="K18" s="12"/>
     </row>
-    <row r="19" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="21"/>
@@ -1802,7 +1801,7 @@
       <c r="J19" s="40"/>
       <c r="K19" s="21"/>
     </row>
-    <row r="20" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="22"/>
       <c r="C20" s="21"/>
@@ -1818,9 +1817,9 @@
       <c r="J20" s="40"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="53" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B21" s="45"/>
       <c r="C21" s="46"/>
@@ -1836,7 +1835,7 @@
       <c r="J21" s="52"/>
       <c r="K21" s="46"/>
     </row>
-    <row r="22" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
       <c r="B22" s="22"/>
       <c r="C22" s="21"/>
@@ -1852,7 +1851,7 @@
       <c r="J22" s="40"/>
       <c r="K22" s="21"/>
     </row>
-    <row r="23" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
       <c r="B23" s="22"/>
       <c r="C23" s="21"/>
@@ -1868,7 +1867,7 @@
       <c r="J23" s="40"/>
       <c r="K23" s="21"/>
     </row>
-    <row r="24" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="22"/>
       <c r="C24" s="21"/>
@@ -1884,7 +1883,7 @@
       <c r="J24" s="40"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
       <c r="B25" s="22"/>
       <c r="C25" s="21"/>
@@ -1900,7 +1899,7 @@
       <c r="J25" s="40"/>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
       <c r="B26" s="22"/>
       <c r="C26" s="21"/>
@@ -1916,7 +1915,7 @@
       <c r="J26" s="40"/>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31"/>
       <c r="B27" s="31"/>
       <c r="C27" s="34"/>
@@ -1932,7 +1931,7 @@
       <c r="J27" s="38"/>
       <c r="K27" s="34"/>
     </row>
-    <row r="28" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="21"/>
@@ -1948,7 +1947,7 @@
       <c r="J28" s="40"/>
       <c r="K28" s="21"/>
     </row>
-    <row r="29" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="31"/>
       <c r="B29" s="31"/>
       <c r="C29" s="34"/>
@@ -1964,7 +1963,7 @@
       <c r="J29" s="38"/>
       <c r="K29" s="34"/>
     </row>
-    <row r="30" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
       <c r="B30" s="31"/>
       <c r="C30" s="34"/>
@@ -1980,7 +1979,7 @@
       <c r="J30" s="38"/>
       <c r="K30" s="34"/>
     </row>
-    <row r="31" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="31"/>
       <c r="B31" s="31"/>
       <c r="C31" s="34"/>
@@ -2123,15 +2122,15 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C31" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"HIGH,MEDIUM,LOW"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,0,-1"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.25"/>
   <pageSetup scale="85" fitToHeight="0" orientation="landscape" r:id="rId2"/>
@@ -2330,19 +2329,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="68.5" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -2351,154 +2350,154 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D5" s="6"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="58"/>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B8" s="61" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D8" s="6"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B9" s="60" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="58"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="59" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="58"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="8"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="8"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="8"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
     </row>
-    <row r="20" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="8"/>
     </row>
-    <row r="22" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B31" s="8"/>
     </row>
-    <row r="32" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="B29" r:id="rId2"/>
-    <hyperlink ref="B9" r:id="rId3"/>
-    <hyperlink ref="B11" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B29" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B9" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B11" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added compliance testing to tasks
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kanes\Documents\Projects\Lightning Trigger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2689F4C4-A791-40F2-8397-517E32D93113}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5F6EB0-6D2C-47FB-BEA1-C5ECAAAC47A8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5568" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTaskList" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
   <si>
     <t>PRIORITY</t>
   </si>
@@ -116,9 +116,6 @@
   <si>
     <t>ACTUAL
 HOURS</t>
-  </si>
-  <si>
-    <t>PROJECT TITLE</t>
   </si>
   <si>
     <t>Project Start</t>
@@ -198,25 +195,62 @@
     <t>SOFTWARE</t>
   </si>
   <si>
-    <t>Draw Schematic</t>
-  </si>
-  <si>
-    <t>Layout PCB</t>
-  </si>
-  <si>
-    <t>Assemble PCB</t>
-  </si>
-  <si>
     <t>Port software off Arduino (To Atmel Studio)</t>
+  </si>
+  <si>
+    <t>TESTING</t>
+  </si>
+  <si>
+    <t>Design testing jig</t>
+  </si>
+  <si>
+    <t>Design software testing</t>
+  </si>
+  <si>
+    <t>Develop Arduino prototype software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design encloosure box cutouts </t>
+  </si>
+  <si>
+    <t>CERTIFICATIION</t>
+  </si>
+  <si>
+    <t>FCC Certification</t>
+  </si>
+  <si>
+    <t>CE Certification</t>
+  </si>
+  <si>
+    <t>UL Certification</t>
+  </si>
+  <si>
+    <t>Draw Prototype Schematic</t>
+  </si>
+  <si>
+    <t>Layout Prototype PCB</t>
+  </si>
+  <si>
+    <t>Assemble Prototype PCB</t>
+  </si>
+  <si>
+    <t>Rework Prototype Schematic</t>
+  </si>
+  <si>
+    <t>Rework Prototype PCB</t>
+  </si>
+  <si>
+    <t>Assemble Rework Prototype PCB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -425,7 +459,7 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -605,6 +639,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -614,6 +660,156 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="37">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -822,156 +1018,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border>
@@ -1147,22 +1193,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table137" displayName="Table137" ref="A5:K31" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A5:K31" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table137" displayName="Table137" ref="A5:K34" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A5:K34" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TASK" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="OWNER" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="PRIORITY" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="START" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="END" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="% COMPLETE" dataDxfId="5" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DONE" dataDxfId="4" dataCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TASK" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="OWNER" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="PRIORITY" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="START" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="END" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="% COMPLETE" dataDxfId="20" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DONE" dataDxfId="19" dataCellStyle="Percent">
       <calculatedColumnFormula>IF(F6&gt;=1,1,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="BUDGET" dataDxfId="3" dataCellStyle="Percent"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="EST._x000a_HOURS" dataDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ACTUAL_x000a_HOURS" dataDxfId="1" dataCellStyle="Percent"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="NOTES" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="BUDGET" dataDxfId="18" dataCellStyle="Percent"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="EST._x000a_HOURS" dataDxfId="17" dataCellStyle="Percent"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ACTUAL_x000a_HOURS" dataDxfId="16" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="NOTES" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="ToDoList" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -1434,15 +1480,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.19921875" customWidth="1"/>
+    <col min="1" max="1" width="35.19921875" customWidth="1"/>
     <col min="2" max="2" width="11.5" customWidth="1"/>
     <col min="3" max="3" width="10.09765625" customWidth="1"/>
     <col min="4" max="4" width="11.09765625" style="20" customWidth="1"/>
@@ -1455,7 +1501,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1470,13 +1516,13 @@
     </row>
     <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H2" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="J2" s="20" t="s">
         <v>29</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>30</v>
       </c>
       <c r="M2" s="23" t="s">
         <v>17</v>
@@ -1484,17 +1530,17 @@
     </row>
     <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="54" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="55">
         <v>42736</v>
       </c>
       <c r="G3" s="54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="56">
         <f>SUM(Table137[BUDGET])</f>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="I3" s="57">
         <f>SUM(Table137[EST.
@@ -1524,10 +1570,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>32</v>
       </c>
       <c r="F5" s="36" t="s">
         <v>15</v>
@@ -1550,7 +1596,7 @@
     </row>
     <row r="6" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="45"/>
       <c r="C6" s="46"/>
@@ -1558,7 +1604,7 @@
       <c r="E6" s="48"/>
       <c r="F6" s="49"/>
       <c r="G6" s="50">
-        <f t="shared" ref="G6:G31" si="0">IF(F6&gt;=1,1,0)</f>
+        <f t="shared" ref="G6:G34" si="0">IF(F6&gt;=1,1,0)</f>
         <v>0</v>
       </c>
       <c r="H6" s="51"/>
@@ -1568,7 +1614,7 @@
     </row>
     <row r="7" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="12" t="s">
@@ -1577,10 +1623,11 @@
       <c r="D7" s="17"/>
       <c r="E7" s="25"/>
       <c r="F7" s="28">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="G7" s="30">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="H7" s="41"/>
       <c r="I7" s="39"/>
@@ -1589,7 +1636,7 @@
     </row>
     <row r="8" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="12" t="s">
@@ -1598,11 +1645,11 @@
       <c r="D8" s="17"/>
       <c r="E8" s="25"/>
       <c r="F8" s="28">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="G8" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="41"/>
       <c r="I8" s="39"/>
@@ -1611,7 +1658,7 @@
     </row>
     <row r="9" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="12" t="s">
@@ -1632,62 +1679,84 @@
       <c r="K9" s="12"/>
     </row>
     <row r="10" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
+      <c r="C10" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="D10" s="17"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="41"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="12"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="28">
+        <v>0</v>
+      </c>
+      <c r="G10" s="33">
+        <f>IF(F10&gt;=1,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="43"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="62"/>
     </row>
     <row r="11" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="50">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="51"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="46"/>
+      <c r="A11" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="28">
+        <v>0</v>
+      </c>
+      <c r="G11" s="33">
+        <f>IF(F11&gt;=1,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="43"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="64"/>
     </row>
     <row r="12" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="41"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="12"/>
+      <c r="C12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="28">
+        <v>0</v>
+      </c>
+      <c r="G12" s="33">
+        <f>IF(F12&gt;=1,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="43"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="65"/>
     </row>
     <row r="13" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="11" t="s">
+        <v>48</v>
+      </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="28"/>
+      <c r="C13" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="28">
+        <v>0</v>
+      </c>
       <c r="G13" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1698,29 +1767,29 @@
       <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="30">
+      <c r="A14" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="45"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="41"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="1:13" s="15" customFormat="1" ht="43.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="51"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="46"/>
+    </row>
+    <row r="15" spans="1:13" s="15" customFormat="1" ht="22.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="11"/>
-      <c r="C15" s="12" t="s">
-        <v>20</v>
-      </c>
+      <c r="C15" s="12"/>
       <c r="D15" s="18"/>
       <c r="E15" s="26"/>
       <c r="F15" s="28">
@@ -1736,22 +1805,20 @@
       <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:13" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="50">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="51"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="46"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="12"/>
     </row>
     <row r="17" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
@@ -1769,71 +1836,89 @@
       <c r="J17" s="39"/>
       <c r="K17" s="12"/>
     </row>
-    <row r="18" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+    <row r="18" spans="1:11" s="15" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
+      <c r="C18" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="D18" s="18"/>
       <c r="E18" s="26"/>
-      <c r="F18" s="28"/>
+      <c r="F18" s="28">
+        <v>0</v>
+      </c>
       <c r="G18" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="42"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
       <c r="K18" s="12"/>
     </row>
     <row r="19" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="30">
+      <c r="A19" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="45"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H19" s="42"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="21"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="46"/>
     </row>
     <row r="20" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="29"/>
+      <c r="A20" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="18"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="28">
+        <v>0</v>
+      </c>
       <c r="G20" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="42"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="21"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="12"/>
     </row>
     <row r="21" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="45"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="50">
+      <c r="A21" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="28">
+        <v>0</v>
+      </c>
+      <c r="G21" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H21" s="51"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="46"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="12"/>
     </row>
     <row r="22" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
@@ -1868,44 +1953,60 @@
       <c r="K23" s="21"/>
     </row>
     <row r="24" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="30">
+      <c r="A24" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="45"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="42"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="21"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="46"/>
     </row>
     <row r="25" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
+      <c r="A25" s="22" t="s">
+        <v>50</v>
+      </c>
       <c r="B25" s="22"/>
-      <c r="C25" s="21"/>
+      <c r="C25" s="21" t="s">
+        <v>20</v>
+      </c>
       <c r="D25" s="19"/>
       <c r="E25" s="27"/>
-      <c r="F25" s="29"/>
+      <c r="F25" s="29">
+        <v>0</v>
+      </c>
       <c r="G25" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H25" s="42"/>
+      <c r="H25" s="42">
+        <v>2000</v>
+      </c>
       <c r="I25" s="40"/>
       <c r="J25" s="40"/>
       <c r="K25" s="21"/>
     </row>
     <row r="26" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+      <c r="A26" s="22" t="s">
+        <v>51</v>
+      </c>
       <c r="B26" s="22"/>
-      <c r="C26" s="21"/>
+      <c r="C26" s="21" t="s">
+        <v>20</v>
+      </c>
       <c r="D26" s="19"/>
       <c r="E26" s="27"/>
-      <c r="F26" s="29"/>
+      <c r="F26" s="29">
+        <v>0</v>
+      </c>
       <c r="G26" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1916,20 +2017,26 @@
       <c r="K26" s="21"/>
     </row>
     <row r="27" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="34"/>
+      <c r="A27" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="22"/>
+      <c r="C27" s="21" t="s">
+        <v>20</v>
+      </c>
       <c r="D27" s="19"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="33">
+      <c r="E27" s="27"/>
+      <c r="F27" s="29">
+        <v>0</v>
+      </c>
+      <c r="G27" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H27" s="43"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="34"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="21"/>
     </row>
     <row r="28" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
@@ -1948,20 +2055,20 @@
       <c r="K28" s="21"/>
     </row>
     <row r="29" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="34"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="21"/>
       <c r="D29" s="19"/>
-      <c r="E29" s="32"/>
+      <c r="E29" s="27"/>
       <c r="F29" s="29"/>
-      <c r="G29" s="33">
+      <c r="G29" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H29" s="43"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
-      <c r="K29" s="34"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="21"/>
     </row>
     <row r="30" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
@@ -1980,23 +2087,71 @@
       <c r="K30" s="34"/>
     </row>
     <row r="31" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="34"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="21"/>
       <c r="D31" s="19"/>
-      <c r="E31" s="32"/>
+      <c r="E31" s="27"/>
       <c r="F31" s="29"/>
-      <c r="G31" s="33">
+      <c r="G31" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H31" s="43"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="34"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="21"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="31"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="43"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="34"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="43"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="34"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="31"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="43"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="34"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F7:F10 F12:F15 F17:F20 F22:F31">
+  <conditionalFormatting sqref="F15:F18 F20:F23 F25:F34 F7:F13">
     <cfRule type="dataBar" priority="24">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2010,14 +2165,14 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:C10 C12:C15 C17:C20 C22:C31">
-    <cfRule type="containsText" dxfId="27" priority="21" operator="containsText" text="LOW">
+  <conditionalFormatting sqref="C15:C18 C20:C23 C25:C34 C7:C13">
+    <cfRule type="containsText" dxfId="14" priority="21" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",C7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="13" priority="22" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",C7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="12" priority="23" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",C7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2036,17 +2191,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="containsText" dxfId="24" priority="16" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",C6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",C6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",C6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
+  <conditionalFormatting sqref="F14">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2060,18 +2215,18 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
-    <cfRule type="containsText" dxfId="21" priority="11" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",C11)))</formula>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",C14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="12" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",C11)))</formula>
+    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",C14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",C11)))</formula>
+    <cfRule type="containsText" dxfId="6" priority="13" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16">
+  <conditionalFormatting sqref="F19">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2085,18 +2240,18 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
-    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",C16)))</formula>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",C19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",C16)))</formula>
+    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",C19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",C16)))</formula>
+    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",C19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F21">
+  <conditionalFormatting sqref="F24">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2110,22 +2265,22 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="LOW">
-      <formula>NOT(ISERROR(SEARCH("LOW",C21)))</formula>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="LOW">
+      <formula>NOT(ISERROR(SEARCH("LOW",C24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="MEDIUM">
-      <formula>NOT(ISERROR(SEARCH("MEDIUM",C21)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="MEDIUM">
+      <formula>NOT(ISERROR(SEARCH("MEDIUM",C24)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="HIGH">
-      <formula>NOT(ISERROR(SEARCH("HIGH",C21)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="HIGH">
+      <formula>NOT(ISERROR(SEARCH("HIGH",C24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C31" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C34" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"HIGH,MEDIUM,LOW"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G31" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G34" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,0,-1"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2137,9 +2292,6 @@
   <headerFooter scaleWithDoc="0">
     <oddFooter>&amp;L&amp;"Arial,Regular"&amp;9&amp;K01+044https://www.vertex42.com/ExcelTemplates/task-list-template.html&amp;R&amp;"Arial,Regular"&amp;9&amp;K01+044Project Task List Template © 2017 by Vertex42.com</oddFooter>
   </headerFooter>
-  <ignoredErrors>
-    <ignoredError sqref="G7" calculatedColumn="1"/>
-  </ignoredErrors>
   <drawing r:id="rId3"/>
   <tableParts count="1">
     <tablePart r:id="rId4"/>
@@ -2161,7 +2313,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F7:F10 F12:F15 F17:F20 F22:F31</xm:sqref>
+          <xm:sqref>F15:F18 F20:F23 F25:F34 F7:F13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{453CAC60-0BFE-49E6-A4CE-35608173DE62}">
@@ -2193,7 +2345,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F11</xm:sqref>
+          <xm:sqref>F14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{43118496-B17C-4230-BC12-D311B22ABA31}">
@@ -2209,7 +2361,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F16</xm:sqref>
+          <xm:sqref>F19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F75D6458-FCC3-457B-9E5E-1B5FC8C89A76}">
@@ -2225,7 +2377,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F21</xm:sqref>
+          <xm:sqref>F24</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="25" id="{4F21F2DD-B176-45C2-9F70-C6C65248398E}">
@@ -2244,7 +2396,7 @@
               <x14:cfIcon iconSet="3Symbols" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>G7:G10 G12:G15 G17:G20 G22:G31</xm:sqref>
+          <xm:sqref>G15:G18 G20:G23 G25:G34 G7:G13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="20" id="{AE261693-65C8-4208-B565-E1A63833ED6C}">
@@ -2282,7 +2434,7 @@
               <x14:cfIcon iconSet="3Symbols" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>G11</xm:sqref>
+          <xm:sqref>G14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="10" id="{BA606E32-70DC-442A-8F86-6A3939739BEF}">
@@ -2301,7 +2453,7 @@
               <x14:cfIcon iconSet="3Symbols" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>G16</xm:sqref>
+          <xm:sqref>G19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="5" id="{B1E307E1-5C3A-42F4-AB76-C279BC1FFE2B}">
@@ -2320,7 +2472,7 @@
               <x14:cfIcon iconSet="3Symbols" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>G21</xm:sqref>
+          <xm:sqref>G24</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2352,7 +2504,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2364,7 +2516,7 @@
     </row>
     <row r="5" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="6"/>
     </row>
@@ -2378,13 +2530,13 @@
     </row>
     <row r="8" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B8" s="61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B9" s="60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="6"/>
     </row>
@@ -2394,7 +2546,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="59" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="6"/>
     </row>
@@ -2415,7 +2567,7 @@
     </row>
     <row r="15" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="6"/>
     </row>
@@ -2432,7 +2584,7 @@
     </row>
     <row r="18" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2448,7 +2600,7 @@
     </row>
     <row r="22" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
more updates to task progress
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -703,156 +703,6 @@
   <dxfs count="37">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1049,6 +899,156 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border>
@@ -1188,7 +1188,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5934CC92-F0EA-465B-8BF0-17665AD69EB8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5934CC92-F0EA-465B-8BF0-17665AD69EB8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1224,22 +1224,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table137" displayName="Table137" ref="A5:K38" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table137" displayName="Table137" ref="A5:K38" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A5:K38"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="TASK" dataDxfId="25"/>
-    <tableColumn id="8" name="OWNER" dataDxfId="24"/>
-    <tableColumn id="7" name="PRIORITY" dataDxfId="23"/>
-    <tableColumn id="4" name="START" dataDxfId="22"/>
-    <tableColumn id="5" name="END" dataDxfId="21"/>
-    <tableColumn id="2" name="% COMPLETE" dataDxfId="20" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="DONE" dataDxfId="19" dataCellStyle="Percent">
+    <tableColumn id="1" name="TASK" dataDxfId="10"/>
+    <tableColumn id="8" name="OWNER" dataDxfId="9"/>
+    <tableColumn id="7" name="PRIORITY" dataDxfId="8"/>
+    <tableColumn id="4" name="START" dataDxfId="7"/>
+    <tableColumn id="5" name="END" dataDxfId="6"/>
+    <tableColumn id="2" name="% COMPLETE" dataDxfId="5" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="DONE" dataDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>IF(F6&gt;=1,1,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="BUDGET" dataDxfId="18" dataCellStyle="Percent"/>
-    <tableColumn id="11" name="EST._x000a_HOURS" dataDxfId="17" dataCellStyle="Percent"/>
-    <tableColumn id="12" name="ACTUAL_x000a_HOURS" dataDxfId="16" dataCellStyle="Percent"/>
-    <tableColumn id="6" name="NOTES" dataDxfId="15"/>
+    <tableColumn id="10" name="BUDGET" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="11" name="EST._x000a_HOURS" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="12" name="ACTUAL_x000a_HOURS" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="6" name="NOTES" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="ToDoList" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -1500,7 +1500,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1514,7 +1514,7 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1862,7 +1862,7 @@
       <c r="D17" s="18"/>
       <c r="E17" s="26"/>
       <c r="F17" s="28">
-        <v>0.6</v>
+        <v>0.95</v>
       </c>
       <c r="G17" s="30">
         <f t="shared" si="0"/>
@@ -1882,7 +1882,7 @@
       <c r="D18" s="18"/>
       <c r="E18" s="63"/>
       <c r="F18" s="68">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="G18" s="33">
         <f>IF(F18&gt;=1,1,0)</f>
@@ -2279,13 +2279,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:C22 C24:C27 C29:C38 C7:C14">
-    <cfRule type="containsText" dxfId="14" priority="21" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="27" priority="21" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",C7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="22" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",C7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="23" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",C7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2304,13 +2304,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="containsText" dxfId="11" priority="16" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="24" priority="16" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",C6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="17" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",C6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="18" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",C6)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2329,13 +2329,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="21" priority="11" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",C15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="20" priority="12" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",C15)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="13" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",C15)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2354,13 +2354,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",C23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="17" priority="7" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",C23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",C23)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2379,13 +2379,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",C28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",C28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",C28)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>